<commit_message>
updated the hi honn go folder
</commit_message>
<xml_diff>
--- a/hi ho nn go/自己积累的/动词变形.xlsx
+++ b/hi ho nn go/自己积累的/动词变形.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Git-repository\CopyFile-master\hi ho nn go\自己积累的\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git-reprository\copyfile\hi ho nn go\自己积累的\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F309AD3-4260-43A6-AA78-1042AC02CAB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C57F4F7C-BAE5-4296-B3CD-77A4F5A96F55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="一类动词" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="243">
   <si>
     <t>基本形</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -981,6 +981,22 @@
   </si>
   <si>
     <t>待たされる</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>書かれる</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>書かせる</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>書かされる</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>書ける</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1322,16 +1338,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="13" width="13.77734375" style="1" customWidth="1"/>
+    <col min="1" max="13" width="13.75" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1372,7 +1388,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -1413,7 +1429,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -1441,8 +1457,20 @@
       <c r="I3" s="1" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="J3" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
@@ -1462,7 +1490,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -1479,7 +1507,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
@@ -1496,7 +1524,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
@@ -1537,7 +1565,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
@@ -1578,7 +1606,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>96</v>
       </c>
@@ -1595,7 +1623,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>97</v>
       </c>
@@ -1612,7 +1640,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>12</v>
       </c>
@@ -1653,17 +1681,17 @@
         <v>219</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>14</v>
       </c>
@@ -1704,7 +1732,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>15</v>
       </c>
@@ -1745,22 +1773,22 @@
         <v>206</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>19</v>
       </c>
@@ -1801,7 +1829,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>20</v>
       </c>
@@ -1842,12 +1870,12 @@
         <v>232</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>22</v>
       </c>
@@ -1864,7 +1892,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>23</v>
       </c>
@@ -1881,62 +1909,62 @@
         <v>81</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>122</v>
       </c>
@@ -1953,7 +1981,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>41</v>
       </c>
@@ -1994,7 +2022,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>99</v>
       </c>
@@ -2026,12 +2054,12 @@
       <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="13" width="13.77734375" style="1" customWidth="1"/>
+    <col min="1" max="13" width="13.75" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2072,7 +2100,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>86</v>
       </c>
@@ -2127,12 +2155,12 @@
       <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="13" width="13.77734375" style="1" customWidth="1"/>
+    <col min="1" max="13" width="13.75" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2173,7 +2201,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>87</v>
       </c>
@@ -2214,7 +2242,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>146</v>
       </c>

</xml_diff>